<commit_message>
Major update to system-wide optimiser
</commit_message>
<xml_diff>
--- a/Compression calculation.xlsx
+++ b/Compression calculation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smros\OneDrive\Documents\00 CAMBRIDGE WORK\09 Thesis\Software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36DF8AF4-15A4-4818-BCBC-7FAF48AE432A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF747317-1951-4758-A065-BC40D993C20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="22620" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -162,13 +162,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,7 +452,7 @@
   <dimension ref="A2:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -473,22 +473,22 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>0.2</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -521,36 +521,36 @@
       </c>
       <c r="B4" s="1">
         <f>B3*100000</f>
-        <v>1300000</v>
+        <v>20000</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>17</v>
       </c>
       <c r="H4">
         <v>250</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="3">
         <f>LOG($B$5,(($H4/I$3)^($B$8/($B$8-1))))*($H4-I$3)*0.83</f>
-        <v>349.30608803200028</v>
-      </c>
-      <c r="J4" s="5">
-        <f t="shared" ref="J4:O4" si="0">LOG($B$5,(($H4/J$3)^($B$8/($B$8-1))))*($H4-J$3)*0.83</f>
-        <v>357.31690527673584</v>
-      </c>
-      <c r="K4" s="5">
+        <v>152.0807399701234</v>
+      </c>
+      <c r="J4" s="3">
+        <f t="shared" ref="J4:L4" si="0">LOG($B$5,(($H4/J$3)^($B$8/($B$8-1))))*($H4-J$3)*0.83</f>
+        <v>155.56848626509552</v>
+      </c>
+      <c r="K4" s="3">
         <f t="shared" si="0"/>
-        <v>365.2046318942397</v>
-      </c>
-      <c r="L4" s="5">
+        <v>159.00264141375166</v>
+      </c>
+      <c r="L4" s="3">
         <f t="shared" si="0"/>
-        <v>372.97724127891547</v>
-      </c>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+        <v>162.38667686924572</v>
+      </c>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
@@ -558,34 +558,34 @@
       </c>
       <c r="B5" s="2">
         <f>B4/B2</f>
-        <v>1625</v>
-      </c>
-      <c r="G5" s="4"/>
+        <v>25</v>
+      </c>
+      <c r="G5" s="5"/>
       <c r="H5">
         <v>260</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I5" s="3">
         <f t="shared" ref="I5:O16" si="1">LOG($B$5,(($H5/I$3)^($B$8/($B$8-1))))*($H5-I$3)*0.83</f>
-        <v>356.44946832081195</v>
-      </c>
-      <c r="J5" s="5">
-        <f t="shared" si="1"/>
-        <v>364.56875461303571</v>
-      </c>
-      <c r="K5" s="5">
-        <f t="shared" si="1"/>
-        <v>372.56247613812576</v>
-      </c>
-      <c r="L5" s="5">
-        <f t="shared" si="1"/>
-        <v>380.43877680319122</v>
-      </c>
-      <c r="M5" s="5">
-        <f t="shared" si="1"/>
-        <v>388.20494773165456</v>
-      </c>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+        <v>155.19082192240521</v>
+      </c>
+      <c r="J5" s="3">
+        <f t="shared" si="1"/>
+        <v>158.7257934263589</v>
+      </c>
+      <c r="K5" s="3">
+        <f t="shared" si="1"/>
+        <v>162.20609659399057</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="1"/>
+        <v>165.6352771162052</v>
+      </c>
+      <c r="M5" s="3">
+        <f t="shared" si="1"/>
+        <v>169.01650939929948</v>
+      </c>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
@@ -597,35 +597,35 @@
       <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="5"/>
       <c r="H6">
         <v>270</v>
       </c>
-      <c r="I6" s="5">
-        <f t="shared" si="1"/>
-        <v>363.50499262181609</v>
-      </c>
-      <c r="J6" s="5">
-        <f t="shared" si="1"/>
-        <v>371.73072016338011</v>
-      </c>
-      <c r="K6" s="5">
-        <f t="shared" si="1"/>
-        <v>379.82844595692933</v>
-      </c>
-      <c r="L6" s="5">
-        <f t="shared" si="1"/>
-        <v>387.80648201545836</v>
-      </c>
-      <c r="M6" s="5">
-        <f t="shared" si="1"/>
-        <v>395.67226936903484</v>
-      </c>
-      <c r="N6" s="5">
-        <f t="shared" si="1"/>
-        <v>403.43250081419046</v>
-      </c>
-      <c r="O6" s="5"/>
+      <c r="I6" s="3">
+        <f t="shared" si="1"/>
+        <v>158.26265317109386</v>
+      </c>
+      <c r="J6" s="3">
+        <f t="shared" si="1"/>
+        <v>161.84396702211117</v>
+      </c>
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
+        <v>165.3695515250796</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="1"/>
+        <v>168.84302556077478</v>
+      </c>
+      <c r="M6" s="3">
+        <f t="shared" si="1"/>
+        <v>172.26762880178663</v>
+      </c>
+      <c r="N6" s="3">
+        <f t="shared" si="1"/>
+        <v>175.64627515509773</v>
+      </c>
+      <c r="O6" s="3"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
@@ -637,37 +637,37 @@
       <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="5"/>
       <c r="H7">
         <v>280</v>
       </c>
-      <c r="I7" s="5">
-        <f t="shared" si="1"/>
-        <v>370.47746280936093</v>
-      </c>
-      <c r="J7" s="5">
-        <f t="shared" si="1"/>
-        <v>378.80772209274585</v>
-      </c>
-      <c r="K7" s="5">
-        <f t="shared" si="1"/>
-        <v>387.00757776872643</v>
-      </c>
-      <c r="L7" s="5">
-        <f t="shared" si="1"/>
-        <v>395.08550767936191</v>
-      </c>
-      <c r="M7" s="5">
-        <f t="shared" si="1"/>
-        <v>403.04910072208082</v>
-      </c>
-      <c r="N7" s="5">
-        <f t="shared" si="1"/>
-        <v>410.90518218701862</v>
-      </c>
-      <c r="O7" s="5">
-        <f t="shared" si="1"/>
-        <v>418.65991726407549</v>
+      <c r="I7" s="3">
+        <f t="shared" si="1"/>
+        <v>161.2983243542549</v>
+      </c>
+      <c r="J7" s="3">
+        <f t="shared" si="1"/>
+        <v>164.92514919174272</v>
+      </c>
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
+        <v>168.49519896063509</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="1"/>
+        <v>172.01216474029738</v>
+      </c>
+      <c r="M7" s="3">
+        <f t="shared" si="1"/>
+        <v>175.47935058174957</v>
+      </c>
+      <c r="N7" s="3">
+        <f t="shared" si="1"/>
+        <v>178.89972807698481</v>
+      </c>
+      <c r="O7" s="3">
+        <f t="shared" si="1"/>
+        <v>182.27598142382899</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.45">
@@ -677,37 +677,37 @@
       <c r="B8">
         <v>1.33</v>
       </c>
-      <c r="G8" s="4"/>
+      <c r="G8" s="5"/>
       <c r="H8">
         <v>290</v>
       </c>
-      <c r="I8" s="5">
-        <f t="shared" si="1"/>
-        <v>377.37125214483115</v>
-      </c>
-      <c r="J8" s="5">
-        <f t="shared" si="1"/>
-        <v>385.80424101433761</v>
-      </c>
-      <c r="K8" s="5">
-        <f t="shared" si="1"/>
-        <v>394.1044576825721</v>
-      </c>
-      <c r="L8" s="5">
-        <f t="shared" si="1"/>
-        <v>402.28054366235796</v>
-      </c>
-      <c r="M8" s="5">
-        <f t="shared" si="1"/>
-        <v>410.34023378545822</v>
-      </c>
-      <c r="N8" s="5">
-        <f t="shared" si="1"/>
-        <v>418.29048409624187</v>
-      </c>
-      <c r="O8" s="5">
-        <f t="shared" si="1"/>
-        <v>426.13757746255931</v>
+      <c r="I8" s="3">
+        <f t="shared" si="1"/>
+        <v>164.29973950061901</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="1"/>
+        <v>167.97129070277521</v>
+      </c>
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
+        <v>171.58503559891858</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="1"/>
+        <v>175.14473652732403</v>
+      </c>
+      <c r="M8" s="3">
+        <f t="shared" si="1"/>
+        <v>178.65376107584177</v>
+      </c>
+      <c r="N8" s="3">
+        <f t="shared" si="1"/>
+        <v>182.11513776418886</v>
+      </c>
+      <c r="O8" s="3">
+        <f t="shared" si="1"/>
+        <v>185.53160202476846</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
@@ -718,37 +718,37 @@
         <f>B7/B6</f>
         <v>1.32</v>
       </c>
-      <c r="G9" s="4"/>
+      <c r="G9" s="5"/>
       <c r="H9">
         <v>300</v>
       </c>
-      <c r="I9" s="5">
-        <f t="shared" si="1"/>
-        <v>384.19035714644565</v>
-      </c>
-      <c r="J9" s="5">
-        <f t="shared" si="1"/>
-        <v>392.72437121494698</v>
-      </c>
-      <c r="K9" s="5">
-        <f t="shared" si="1"/>
-        <v>401.12327605750897</v>
-      </c>
-      <c r="L9" s="5">
-        <f t="shared" si="1"/>
-        <v>409.3958748078295</v>
-      </c>
-      <c r="M9" s="5">
-        <f t="shared" si="1"/>
-        <v>417.55004639617687</v>
-      </c>
-      <c r="N9" s="5">
-        <f t="shared" si="1"/>
-        <v>425.59287596932728</v>
-      </c>
-      <c r="O9" s="5">
-        <f t="shared" si="1"/>
-        <v>433.53076258041631</v>
+      <c r="I9" s="3">
+        <f t="shared" si="1"/>
+        <v>167.26863861263365</v>
+      </c>
+      <c r="J9" s="3">
+        <f t="shared" si="1"/>
+        <v>170.98417412409665</v>
+      </c>
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>174.64088583671492</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="1"/>
+        <v>178.24260645519269</v>
+      </c>
+      <c r="M9" s="3">
+        <f t="shared" si="1"/>
+        <v>181.79276630492771</v>
+      </c>
+      <c r="N9" s="3">
+        <f t="shared" si="1"/>
+        <v>185.2944501141898</v>
+      </c>
+      <c r="O9" s="3">
+        <f t="shared" si="1"/>
+        <v>188.75044390008324</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">
@@ -759,37 +759,37 @@
         <f>B9^(B8/(B8-1))</f>
         <v>3.0616072688317431</v>
       </c>
-      <c r="G10" s="4"/>
+      <c r="G10" s="5"/>
       <c r="H10">
         <v>310</v>
       </c>
-      <c r="I10" s="5">
-        <f t="shared" si="1"/>
-        <v>390.93844165325839</v>
-      </c>
-      <c r="J10" s="5">
-        <f t="shared" si="1"/>
-        <v>399.57186586690807</v>
-      </c>
-      <c r="K10" s="5">
-        <f t="shared" si="1"/>
-        <v>408.06787384385041</v>
-      </c>
-      <c r="L10" s="5">
-        <f t="shared" si="1"/>
-        <v>416.43542838824629</v>
-      </c>
-      <c r="M10" s="5">
-        <f t="shared" si="1"/>
-        <v>424.68255078221932</v>
-      </c>
-      <c r="N10" s="5">
-        <f t="shared" si="1"/>
-        <v>432.81645370344688</v>
-      </c>
-      <c r="O10" s="5">
-        <f t="shared" si="1"/>
-        <v>440.843650970336</v>
+      <c r="I10" s="3">
+        <f t="shared" si="1"/>
+        <v>170.20661685102894</v>
+      </c>
+      <c r="J10" s="3">
+        <f t="shared" si="1"/>
+        <v>173.96543351032386</v>
+      </c>
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
+        <v>177.66442194538115</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" si="1"/>
+        <v>181.30748437816507</v>
+      </c>
+      <c r="M10" s="3">
+        <f t="shared" si="1"/>
+        <v>184.89811311116526</v>
+      </c>
+      <c r="N10" s="3">
+        <f t="shared" si="1"/>
+        <v>188.43944839700228</v>
+      </c>
+      <c r="O10" s="3">
+        <f t="shared" si="1"/>
+        <v>191.93432621923716</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.45">
@@ -798,39 +798,39 @@
       </c>
       <c r="B11">
         <f>LOG(B5,B10)</f>
-        <v>6.6073810043730576</v>
-      </c>
-      <c r="G11" s="4"/>
+        <v>2.876718805764233</v>
+      </c>
+      <c r="G11" s="5"/>
       <c r="H11">
         <v>320</v>
       </c>
-      <c r="I11" s="5">
-        <f t="shared" si="1"/>
-        <v>397.61887447260483</v>
-      </c>
-      <c r="J11" s="5">
-        <f t="shared" si="1"/>
-        <v>406.35017565335266</v>
-      </c>
-      <c r="K11" s="5">
-        <f t="shared" si="1"/>
-        <v>414.94178217032055</v>
-      </c>
-      <c r="L11" s="5">
-        <f t="shared" si="1"/>
-        <v>423.40281463926965</v>
-      </c>
-      <c r="M11" s="5">
-        <f t="shared" si="1"/>
-        <v>431.74143502959453</v>
-      </c>
-      <c r="N11" s="5">
-        <f t="shared" si="1"/>
-        <v>439.96498205227772</v>
-      </c>
-      <c r="O11" s="5">
-        <f t="shared" si="1"/>
-        <v>448.08008293782899</v>
+      <c r="I11" s="3">
+        <f t="shared" si="1"/>
+        <v>173.11514092574768</v>
+      </c>
+      <c r="J11" s="3">
+        <f t="shared" si="1"/>
+        <v>176.91657121844989</v>
+      </c>
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
+        <v>180.65718130627894</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="1"/>
+        <v>184.34094211914845</v>
+      </c>
+      <c r="M11" s="3">
+        <f t="shared" si="1"/>
+        <v>187.97140721191371</v>
+      </c>
+      <c r="N11" s="3">
+        <f t="shared" si="1"/>
+        <v>191.55177170952359</v>
+      </c>
+      <c r="O11" s="3">
+        <f t="shared" si="1"/>
+        <v>195.0849209728533</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.45">
@@ -839,76 +839,76 @@
       </c>
       <c r="B12">
         <f>(B7-B6)*B11*0.83</f>
-        <v>438.73009869037099</v>
+        <v>191.01412870274507</v>
       </c>
       <c r="C12" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="4"/>
+      <c r="G12" s="5"/>
       <c r="H12">
         <v>330</v>
       </c>
-      <c r="I12" s="5">
-        <f t="shared" si="1"/>
-        <v>404.23476171724326</v>
-      </c>
-      <c r="J12" s="5">
-        <f t="shared" si="1"/>
-        <v>413.0624819427544</v>
-      </c>
-      <c r="K12" s="5">
-        <f t="shared" si="1"/>
-        <v>421.74825634232349</v>
-      </c>
-      <c r="L12" s="5">
-        <f t="shared" si="1"/>
-        <v>430.30136156892593</v>
-      </c>
-      <c r="M12" s="5">
-        <f t="shared" si="1"/>
-        <v>438.73009869037099</v>
-      </c>
-      <c r="N12" s="5">
-        <f t="shared" si="1"/>
-        <v>447.04193102154369</v>
-      </c>
-      <c r="O12" s="5">
-        <f t="shared" si="1"/>
-        <v>455.24359791356341</v>
+      <c r="I12" s="3">
+        <f t="shared" si="1"/>
+        <v>175.99556317487648</v>
+      </c>
+      <c r="J12" s="3">
+        <f t="shared" si="1"/>
+        <v>179.83897235136351</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" si="1"/>
+        <v>183.62058121292731</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="1"/>
+        <v>187.34442862489936</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="1"/>
+        <v>191.01412870274507</v>
+      </c>
+      <c r="N12" s="3">
+        <f t="shared" si="1"/>
+        <v>194.63293082140882</v>
+      </c>
+      <c r="O12" s="3">
+        <f t="shared" si="1"/>
+        <v>198.20376915679029</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="G13" s="4"/>
+      <c r="G13" s="5"/>
       <c r="H13">
         <v>340</v>
       </c>
-      <c r="I13" s="5">
-        <f t="shared" si="1"/>
-        <v>410.78897471993139</v>
-      </c>
-      <c r="J13" s="5">
-        <f t="shared" si="1"/>
-        <v>419.71172542431088</v>
-      </c>
-      <c r="K13" s="5">
-        <f t="shared" si="1"/>
-        <v>428.49030518631412</v>
-      </c>
-      <c r="L13" s="5">
-        <f t="shared" si="1"/>
-        <v>437.13414499989938</v>
-      </c>
-      <c r="M13" s="5">
-        <f t="shared" si="1"/>
-        <v>445.65168351248639</v>
-      </c>
-      <c r="N13" s="5">
-        <f t="shared" si="1"/>
-        <v>454.05050727654447</v>
-      </c>
-      <c r="O13" s="5">
-        <f t="shared" si="1"/>
-        <v>462.33746652936367</v>
+      <c r="I13" s="3">
+        <f t="shared" si="1"/>
+        <v>178.84913371808244</v>
+      </c>
+      <c r="J13" s="3">
+        <f t="shared" si="1"/>
+        <v>182.73391722510979</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="1"/>
+        <v>186.55593164694233</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="1"/>
+        <v>190.31928304582442</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="1"/>
+        <v>194.02764543657548</v>
+      </c>
+      <c r="N13" s="3">
+        <f t="shared" si="1"/>
+        <v>197.68432184926829</v>
+      </c>
+      <c r="O13" s="3">
+        <f t="shared" si="1"/>
+        <v>201.29229473737772</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.45">
@@ -921,37 +921,37 @@
       <c r="D14" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="4"/>
+      <c r="G14" s="5"/>
       <c r="H14">
         <v>350</v>
       </c>
-      <c r="I14" s="5">
-        <f t="shared" si="1"/>
-        <v>417.2841742429847</v>
-      </c>
-      <c r="J14" s="5">
-        <f t="shared" si="1"/>
-        <v>426.30063094089132</v>
-      </c>
-      <c r="K14" s="5">
-        <f t="shared" si="1"/>
-        <v>435.17071649588661</v>
-      </c>
-      <c r="L14" s="5">
-        <f t="shared" si="1"/>
-        <v>443.90401461915661</v>
-      </c>
-      <c r="M14" s="5">
-        <f t="shared" si="1"/>
-        <v>452.50910008388735</v>
-      </c>
-      <c r="N14" s="5">
-        <f t="shared" si="1"/>
-        <v>460.9936813723121</v>
-      </c>
-      <c r="O14" s="5">
-        <f t="shared" si="1"/>
-        <v>469.36471842635029</v>
+      <c r="I14" s="3">
+        <f t="shared" si="1"/>
+        <v>181.67701099696069</v>
+      </c>
+      <c r="J14" s="3">
+        <f t="shared" si="1"/>
+        <v>185.60259218064903</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>189.46444635674462</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="1"/>
+        <v>193.26674607745525</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="1"/>
+        <v>197.01322462398005</v>
+      </c>
+      <c r="N14" s="3">
+        <f t="shared" si="1"/>
+        <v>200.70723811212201</v>
+      </c>
+      <c r="O14" s="3">
+        <f t="shared" si="1"/>
+        <v>204.35181675851197</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.45">
@@ -967,37 +967,37 @@
       <c r="D15">
         <v>0.78</v>
       </c>
-      <c r="G15" s="4"/>
+      <c r="G15" s="5"/>
       <c r="H15">
         <v>360</v>
       </c>
-      <c r="I15" s="5">
-        <f t="shared" si="1"/>
-        <v>423.72283156673677</v>
-      </c>
-      <c r="J15" s="5">
-        <f t="shared" si="1"/>
-        <v>432.83172911904722</v>
-      </c>
-      <c r="K15" s="5">
-        <f t="shared" si="1"/>
-        <v>441.79207919440285</v>
-      </c>
-      <c r="L15" s="5">
-        <f t="shared" si="1"/>
-        <v>450.61361666482298</v>
-      </c>
-      <c r="M15" s="5">
-        <f t="shared" si="1"/>
-        <v>459.30505103579446</v>
-      </c>
-      <c r="N15" s="5">
-        <f t="shared" si="1"/>
-        <v>467.87421146585683</v>
-      </c>
-      <c r="O15" s="5">
-        <f t="shared" si="1"/>
-        <v>476.32816646917837</v>
+      <c r="I15" s="3">
+        <f t="shared" si="1"/>
+        <v>184.48027095651958</v>
+      </c>
+      <c r="J15" s="3">
+        <f t="shared" si="1"/>
+        <v>188.44609900112133</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="1"/>
+        <v>192.34725250671551</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="1"/>
+        <v>196.18796983785111</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="1"/>
+        <v>199.97204293542049</v>
+      </c>
+      <c r="N15" s="3">
+        <f t="shared" si="1"/>
+        <v>203.7028804552269</v>
+      </c>
+      <c r="O15" s="3">
+        <f t="shared" si="1"/>
+        <v>207.383559884042</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.45">
@@ -1016,37 +1016,37 @@
         <f t="shared" si="2"/>
         <v>2.393539476367565</v>
       </c>
-      <c r="G16" s="4"/>
+      <c r="G16" s="5"/>
       <c r="H16">
         <v>370</v>
       </c>
-      <c r="I16" s="5">
-        <f t="shared" si="1"/>
-        <v>430.10724693510036</v>
-      </c>
-      <c r="J16" s="5">
-        <f t="shared" si="1"/>
-        <v>439.30737528700121</v>
-      </c>
-      <c r="K16" s="5">
-        <f t="shared" si="1"/>
-        <v>448.35680271759185</v>
-      </c>
-      <c r="L16" s="5">
-        <f t="shared" si="1"/>
-        <v>457.26541376607713</v>
-      </c>
-      <c r="M16" s="5">
-        <f t="shared" si="1"/>
-        <v>466.04205133300849</v>
-      </c>
-      <c r="N16" s="5">
-        <f t="shared" si="1"/>
-        <v>474.69466405040737</v>
-      </c>
-      <c r="O16" s="5">
-        <f t="shared" si="1"/>
-        <v>483.23042791809485</v>
+      <c r="I16" s="3">
+        <f t="shared" si="1"/>
+        <v>187.25991507600145</v>
+      </c>
+      <c r="J16" s="3">
+        <f t="shared" si="1"/>
+        <v>191.26546314835289</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="1"/>
+        <v>195.20539911598502</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="1"/>
+        <v>199.08402650548399</v>
+      </c>
+      <c r="M16" s="3">
+        <f t="shared" si="1"/>
+        <v>202.90519533523033</v>
+      </c>
+      <c r="N16" s="3">
+        <f t="shared" si="1"/>
+        <v>206.67236627734221</v>
+      </c>
+      <c r="O16" s="3">
+        <f t="shared" si="1"/>
+        <v>210.38866361565036</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
@@ -1055,15 +1055,15 @@
       </c>
       <c r="B17">
         <f>LOG($B$5,B16)</f>
-        <v>7.4240236004191669</v>
+        <v>3.2322683210834082</v>
       </c>
       <c r="C17">
         <f t="shared" ref="C17:D17" si="3">LOG($B$5,C16)</f>
-        <v>7.9607000052687438</v>
+        <v>3.4659262720051003</v>
       </c>
       <c r="D17">
         <f t="shared" si="3"/>
-        <v>8.4710012876577672</v>
+        <v>3.6881010330310682</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
@@ -1074,7 +1074,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C18">
-        <v>2.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D18">
         <v>5</v>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="C19">
         <f t="shared" ref="C19:D19" si="4">LOG($B$10,C18)</f>
-        <v>1.2781039248783796</v>
+        <v>1.4191509719731503</v>
       </c>
       <c r="D19">
         <f t="shared" si="4"/>

</xml_diff>